<commit_message>
Write First Row With Right Format
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,25 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>sub_title</t>
-  </si>
-  <si>
-    <t>Supervisor_Section</t>
-  </si>
-  <si>
-    <t>Employees</t>
+    <t>Personal Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,21 +34,6 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -84,19 +60,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -392,7 +359,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,51 +369,39 @@
     <col min="2" max="26" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="50.25" customHeight="1">
+    <row r="1" spans="2:17" ht="50.25" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="33.75" customHeight="1">
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="33.75" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="2" spans="2:17" ht="33.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:D1"/>
+  <mergeCells count="4">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Second Row Finished (Remaining Data Structure For Employee/Supervisor)
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,16 +14,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Personal Data</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>join_date</t>
+  </si>
+  <si>
+    <t>supervisor_rating</t>
+  </si>
+  <si>
+    <t>clients_rating</t>
+  </si>
+  <si>
+    <t>ai_rating</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,6 +61,14 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -60,9 +95,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -366,10 +404,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="26" width="15" customWidth="1"/>
+    <col min="2" max="26" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="50.25" customHeight="1">
+    <row r="1" spans="1:17" ht="50.25" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -395,7 +433,59 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="2:17" ht="33.75" customHeight="1"/>
+    <row r="2" spans="1:17" ht="33.75" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:E1"/>

</xml_diff>

<commit_message>
All Finished, Optimizing the Code
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Personal Data</t>
   </si>
@@ -44,13 +44,37 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>Supervisor_2</t>
+  </si>
+  <si>
+    <t>__</t>
+  </si>
+  <si>
+    <t>employee_3</t>
+  </si>
+  <si>
+    <t>employee_4</t>
+  </si>
+  <si>
+    <t>Supervisor_1</t>
+  </si>
+  <si>
+    <t>employee_1</t>
+  </si>
+  <si>
+    <t>employee_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +92,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -95,13 +126,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -397,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,6 +524,168 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:17" ht="33.75" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3" s="4">
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>23</v>
+      </c>
+      <c r="E4" s="4">
+        <v>40909</v>
+      </c>
+      <c r="N4">
+        <v>7.3</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>23</v>
+      </c>
+      <c r="E5" s="4">
+        <v>40909</v>
+      </c>
+      <c r="N5">
+        <v>2.5</v>
+      </c>
+      <c r="O5">
+        <v>2.4</v>
+      </c>
+      <c r="P5">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="33.75" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4">
+        <v>44197</v>
+      </c>
+      <c r="F6">
+        <v>9.5</v>
+      </c>
+      <c r="G6">
+        <v>8.6</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6" s="4">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>22</v>
+      </c>
+      <c r="E7" s="4">
+        <v>44562</v>
+      </c>
+      <c r="F7">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="G7">
+        <v>8.6</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7" s="4">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4">
+        <v>40909</v>
+      </c>
+      <c r="J8">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>8</v>
+      </c>
+      <c r="M8" s="4">
+        <v>44197</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:E1"/>

</xml_diff>